<commit_message>
comments on old template
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
+++ b/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
@@ -940,7 +940,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -963,7 +963,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>

</xml_diff>

<commit_message>
LBS empirical measurement template updated measures
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
+++ b/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="273">
   <si>
     <t xml:space="preserve">Sfwr Name</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">small personal blog project, no clear docs (likely red but double check)</t>
+    <t xml:space="preserve">small personal blog project, no clear docs, no mention of installation</t>
   </si>
   <si>
     <t xml:space="preserve">Atruszkowska/LBM_MATLAB</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">HDF5, Cmake</t>
   </si>
   <si>
-    <t xml:space="preserve">no docs, no installation guide (consider contacting the devs)</t>
+    <t xml:space="preserve">no docs, no installation guide, small project</t>
   </si>
   <si>
     <t xml:space="preserve">CUDA-LBM-simulator</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">Nvidia NSight and OpenGL</t>
   </si>
   <si>
-    <t xml:space="preserve">Small school project, is running possible?</t>
+    <t xml:space="preserve">Small school project, need CUDA, dead</t>
   </si>
   <si>
     <t xml:space="preserve">CudneLB (TCLB)</t>
@@ -260,7 +260,7 @@
     <t xml:space="preserve">NVIDIA CUDA</t>
   </si>
   <si>
-    <t xml:space="preserve">website but no clear way to get the code; website states that the software is in development and considered a prototype</t>
+    <t xml:space="preserve">There is a website but not clear way to get the code; website states that the software is in development and considered a prototype</t>
   </si>
   <si>
     <t xml:space="preserve">eLBM</t>
@@ -344,7 +344,7 @@
     <t xml:space="preserve">Unfinished finite volume LBM solver</t>
   </si>
   <si>
-    <t xml:space="preserve">Personal project, dead, marked as incomplete, unclear how to install and run</t>
+    <t xml:space="preserve">Personal project, dead, unclear how to install and run</t>
   </si>
   <si>
     <t xml:space="preserve">HemeLB</t>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">Java</t>
   </si>
   <si>
-    <t xml:space="preserve">no docs, small project, 10 years since any code changes</t>
+    <t xml:space="preserve">no docs, small project, 10 years since any code changes, dead</t>
   </si>
   <si>
     <t xml:space="preserve">laboetie</t>
@@ -485,7 +485,7 @@
     <t xml:space="preserve">supporting complex boundaries</t>
   </si>
   <si>
-    <t xml:space="preserve">no docs or installation guide; small project; inactive for 5 years</t>
+    <t xml:space="preserve">no docs or installation guide; personal project; inactive for 5 years</t>
   </si>
   <si>
     <t xml:space="preserve">lettuce</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">Cmake, VDKFortran</t>
   </si>
   <si>
-    <t xml:space="preserve">School project, 1 days worth of commits, might be able to run it..decide on second pass</t>
+    <t xml:space="preserve">School project, 1 days worth of commits, repeat problems with VTK (requirement) when attempting test installation, dead</t>
   </si>
   <si>
     <t xml:space="preserve">loliverhennigh</t>
@@ -557,6 +557,9 @@
     <t xml:space="preserve">D2Q5, D3Q15, D3Q19</t>
   </si>
   <si>
+    <t xml:space="preserve">personal project, no docs, dead</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ludwig</t>
   </si>
   <si>
@@ -626,6 +629,12 @@
     <t xml:space="preserve">openLBMflow</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/wme7/openLBMflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dead for 6 years, no user guide, linked website no longer works, small project</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palabos</t>
   </si>
   <si>
@@ -662,12 +671,18 @@
     <t xml:space="preserve">MIT</t>
   </si>
   <si>
+    <t xml:space="preserve">dead for 4 years, unclear documentation, unclear installation on non-CUDA, do not have CUDA to run CUDA version, even CUDA docs are unclear and in many places</t>
+  </si>
+  <si>
     <t xml:space="preserve">PowerFLOW</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.3ds.com/products-services/simulia/products/powerflow/</t>
   </si>
   <si>
+    <t xml:space="preserve">not open source, need to purchase commercial license</t>
+  </si>
+  <si>
     <t xml:space="preserve">ProLB</t>
   </si>
   <si>
@@ -728,6 +743,9 @@
     <t xml:space="preserve">Curved Boundaries </t>
   </si>
   <si>
+    <t xml:space="preserve">no installation instructions or user manual, personal project, dead</t>
+  </si>
+  <si>
     <t xml:space="preserve">SunlightLB</t>
   </si>
   <si>
@@ -752,6 +770,9 @@
     <t xml:space="preserve">Lattice Boltzmann code from LANL , Shan and Chen Lattice Boltzmann Method </t>
   </si>
   <si>
+    <t xml:space="preserve">problems installing dependency needed before installation; could not even begin installing solver, broken link to some docs</t>
+  </si>
+  <si>
     <t xml:space="preserve">turbulent_lbm_multigpu</t>
   </si>
   <si>
@@ -767,6 +788,9 @@
     <t xml:space="preserve">Apache License, Version 2.0 </t>
   </si>
   <si>
+    <t xml:space="preserve">Dead 7 years, no clear way to install</t>
+  </si>
+  <si>
     <t xml:space="preserve">waLBerla</t>
   </si>
   <si>
@@ -797,6 +821,9 @@
     <t xml:space="preserve">1D, 2D</t>
   </si>
   <si>
+    <t xml:space="preserve">dead, unclear how to run examples, cannot find docs, personal project</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zmhhaha/LBM-Cplusplus-A.A.Mohamad</t>
   </si>
   <si>
@@ -810,6 +837,9 @@
   </si>
   <si>
     <t xml:space="preserve">C++ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">personal project, unclear how to run, little documentation</t>
   </si>
 </sst>
 </file>
@@ -870,18 +900,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -897,8 +921,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFC9211E"/>
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -936,7 +960,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -961,6 +985,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -969,15 +997,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -993,39 +1017,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,7 +1104,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1131,11 +1123,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
@@ -1253,41 +1245,41 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+    <row r="3" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1319,7 +1311,7 @@
       <c r="L4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -1331,735 +1323,735 @@
       <c r="Q4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="R4" s="6" t="s">
         <v>44</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+    <row r="5" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" s="11" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
+    <row r="6" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="11" t="n">
+      <c r="E6" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="F6" s="11" t="n">
+      <c r="F6" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+    <row r="7" s="11" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="11" t="n">
         <v>141</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="11" t="n">
         <v>2020</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
+    <row r="8" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="15" t="n">
+      <c r="E8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="15" t="n">
+      <c r="F8" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="N8" s="15" t="s">
+      <c r="L8" s="6"/>
+      <c r="N8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="17" t="s">
+      <c r="R8" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="W8" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+    <row r="9" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="15" t="n">
+      <c r="E9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="15" t="n">
+      <c r="F9" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R9" s="17"/>
-      <c r="W9" s="15" t="s">
+      <c r="R9" s="6"/>
+      <c r="W9" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" s="11" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="n">
+    <row r="10" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="11" t="n">
+      <c r="E10" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="N10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="R10" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="n">
+    <row r="11" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="11" t="n">
+      <c r="E11" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="F11" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="R11" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+    <row r="12" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="15" t="n">
+      <c r="E12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="15" t="s">
+      <c r="R12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="W12" s="15" t="s">
+      <c r="W12" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
+    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="15" t="n">
+      <c r="E13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="15" t="s">
+      <c r="W13" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" s="11" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="n">
+    <row r="14" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="11" t="n">
+      <c r="E14" s="7" t="n">
         <v>208</v>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="F14" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="N14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
+    <row r="15" s="2" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="15" t="n">
+      <c r="E15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="15" t="n">
+      <c r="F15" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="W15" s="15" t="s">
+      <c r="W15" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="n">
+    <row r="16" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="F16" s="7" t="n">
         <v>2018</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="N16" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="n">
+    <row r="17" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="11" t="n">
+      <c r="E17" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="F17" s="7" t="n">
         <v>2015</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="M17" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" s="11" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="n">
+    <row r="18" s="7" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="11" t="n">
+      <c r="C18" s="7" t="n">
         <v>2012</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E18" s="11" t="n">
+      <c r="E18" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="F18" s="7" t="n">
         <v>2016</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" s="11" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="n">
+    <row r="19" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="11" t="n">
+      <c r="E19" s="7" t="n">
         <v>142</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="F19" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
+    <row r="20" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E20" s="15" t="n">
+      <c r="E20" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F20" s="15" t="n">
+      <c r="F20" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="17"/>
-      <c r="N20" s="15" t="s">
+      <c r="M20" s="6"/>
+      <c r="N20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="W20" s="15" t="s">
+      <c r="W20" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" s="11" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="n">
+    <row r="21" s="7" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="11" t="n">
+      <c r="E21" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="F21" s="11" t="n">
+      <c r="F21" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="11" t="s">
+      <c r="M21" s="9"/>
+      <c r="N21" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+    <row r="22" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="15" t="n">
+      <c r="E22" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="F22" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="W22" s="15" t="s">
+      <c r="W22" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="n">
+    <row r="23" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="11" t="n">
+      <c r="E23" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="M23" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="R23" s="11" t="s">
+      <c r="R23" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="24" s="11" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="n">
+    <row r="24" s="7" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="11" t="n">
+      <c r="C24" s="7" t="n">
         <v>2014</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="11" t="n">
+      <c r="E24" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F24" s="11" t="n">
+      <c r="F24" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="11" t="s">
+      <c r="L24" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="M24" s="11" t="s">
+      <c r="M24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="7" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2107,627 +2099,660 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="n">
+    <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="15" t="n">
+      <c r="E26" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="W26" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="B27" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="0" t="n">
+      <c r="D27" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="7" t="n">
         <v>2018</v>
       </c>
-      <c r="G27" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="L27" s="0" t="s">
+      <c r="G27" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="L27" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N27" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+    <row r="28" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="B28" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="E28" s="0" t="n">
+      <c r="D28" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="7" t="n">
         <v>2019</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="H28" s="0" t="s">
+      <c r="G28" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="N28" s="0" t="s">
+      <c r="L28" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="N28" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+    <row r="29" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="B29" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="D29" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="7" t="n">
         <v>2018</v>
       </c>
-      <c r="G29" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="H29" s="0" t="s">
+      <c r="G29" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="0" t="s">
+      <c r="L29" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="B30" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="C30" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="D30" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="7" t="n">
         <v>2017</v>
       </c>
-      <c r="G30" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="H30" s="0" t="s">
+      <c r="G30" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="L30" s="0" t="s">
+      <c r="L30" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="M30" s="0" t="s">
+      <c r="M30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N30" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="R30" s="0" t="s">
+      <c r="N30" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="R30" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+    <row r="31" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="F31" s="7" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E31" s="0" t="n">
+    </row>
+    <row r="32" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>672</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="L34" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="W35" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="W36" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R37" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <v>2020</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="R38" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" s="7" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E40" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="F40" s="7" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M40" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="F31" s="0" t="n">
+    </row>
+    <row r="41" s="2" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="E43" s="7" t="n">
+        <v>454</v>
+      </c>
+      <c r="F43" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G31" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="H31" s="0" t="s">
+      <c r="G43" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="L31" s="0" t="s">
+      <c r="I43" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" s="2" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="N31" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="32" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>672</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I33" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="N33" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>2017</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="21"/>
-      <c r="L34" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="M34" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="N34" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E35" s="15" t="n">
-        <v>12</v>
-      </c>
-      <c r="F35" s="15" t="n">
-        <v>2018</v>
-      </c>
-      <c r="G35" s="17"/>
-      <c r="I35" s="17"/>
-    </row>
-    <row r="36" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F36" s="15" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="H36" s="15" t="s">
+      <c r="W44" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" s="2" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I36" s="17"/>
-    </row>
-    <row r="37" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="E37" s="11" t="n">
-        <v>11</v>
-      </c>
-      <c r="F37" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="L37" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="N37" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="R37" s="13" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L38" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="M38" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="N38" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="R38" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L39" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G40" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="M40" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="L41" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="M41" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="L42" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="O42" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>454</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="L43" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="M43" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N43" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="R43" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="G44" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="L44" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L45" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="M45" s="0" t="s">
+      <c r="L45" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>131</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
measured LBM solver DL_MESO and added to empirical measures table
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
+++ b/StateOfPractice/Peter-Notes/Peter-SolverSolutions_filtered.xlsx
@@ -900,7 +900,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,12 +917,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -960,7 +954,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1002,18 +996,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1076,7 +1058,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -1104,7 +1086,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1123,11 +1105,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
@@ -1415,47 +1397,47 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" s="11" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="n">
+    <row r="7" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="11" t="n">
+      <c r="E7" s="7" t="n">
         <v>141</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="7" t="n">
         <v>2020</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="11" t="s">
+      <c r="W7" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1582,7 +1564,7 @@
       <c r="C11" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="7" t="n">
@@ -2324,7 +2306,7 @@
       <c r="C33" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="11" t="s">
         <v>206</v>
       </c>
       <c r="E33" s="7" t="n">
@@ -2669,7 +2651,7 @@
       <c r="C43" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="11" t="s">
         <v>257</v>
       </c>
       <c r="E43" s="7" t="n">

</xml_diff>